<commit_message>
add sequential method for tree
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/SequentialExecutionTimes.xlsx
+++ b/src/main/resources/data_output/SequentialExecutionTimes.xlsx
@@ -7723,7 +7723,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -8046,6 +8046,12 @@
       </c>
     </row>
     <row r="23">
+      <c r="A23" t="n">
+        <v>0.0312288</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.0293721</v>
+      </c>
       <c r="C23" t="n">
         <v>0.0033707</v>
       </c>
@@ -8054,6 +8060,12 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="n">
+        <v>0.0213415</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.021437</v>
+      </c>
       <c r="C24" t="n">
         <v>0.0040288</v>
       </c>
@@ -8075,6 +8087,30 @@
       </c>
       <c r="D26" t="n">
         <v>0.0020525</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="n">
+        <v>0.0072541</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0037323</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="n">
+        <v>0.0201335</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0077251</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="n">
+        <v>0.0092403</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0047571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored code for ExcelDataRecorder
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/SequentialExecutionTimes.xlsx
+++ b/src/main/resources/data_output/SequentialExecutionTimes.xlsx
@@ -8074,6 +8074,12 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="n">
+        <v>0.032607</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.0247385</v>
+      </c>
       <c r="C25" t="n">
         <v>0.0127245</v>
       </c>
@@ -8082,6 +8088,12 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="n">
+        <v>0.0237495</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.0236449</v>
+      </c>
       <c r="C26" t="n">
         <v>0.0043228</v>
       </c>

</xml_diff>

<commit_message>
added classes for parallel implementation for trees
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/SequentialExecutionTimes.xlsx
+++ b/src/main/resources/data_output/SequentialExecutionTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anul1 IS1.1 Semestrul2\MEvPerf\SearchAlgorithms\src\main\resources\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C9E7ED-51F7-440C-ADD2-891E64F4EBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210FD9E6-78C0-480A-9E9D-F3C38A6886E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,15 +68,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -84,18 +108,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,6 +181,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time Execution For Graph 10000</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -203,10 +281,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$A$2:$A$4</c:f>
+              <c:f>'Execution Times'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2.74994E-2</c:v>
                 </c:pt>
@@ -215,6 +293,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.5272400000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7387600000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.91285E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -266,10 +350,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$B$2:$B$4</c:f>
+              <c:f>'Execution Times'!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2.4012100000000001E-2</c:v>
                 </c:pt>
@@ -278,6 +362,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.6511300000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2605699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9986400000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,6 +596,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time Execution For Graph 1000</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -581,10 +701,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$C$2:$C$4</c:f>
+              <c:f>'Execution Times'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4.8685000000000004E-3</c:v>
                 </c:pt>
@@ -593,6 +713,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.2054000000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.10049E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.07534E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -644,10 +770,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$D$2:$D$4</c:f>
+              <c:f>'Execution Times'!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>3.4110009999999999E-3</c:v>
                 </c:pt>
@@ -656,6 +782,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.9805999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2648E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0403000000000002E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,6 +1016,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time Execution For Tree 10000</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -959,10 +1121,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$E$2:$E$4</c:f>
+              <c:f>'Execution Times'!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>7.8680000000000004E-4</c:v>
                 </c:pt>
@@ -971,6 +1133,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.008E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4400000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.47E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1022,10 +1190,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$F$2:$F$4</c:f>
+              <c:f>'Execution Times'!$F$2:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>7.7220000000000001E-4</c:v>
                 </c:pt>
@@ -1034,6 +1202,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0450000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5800000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8100000000000001E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1262,6 +1436,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time Execution For Tree 1000</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1337,10 +1541,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$G$2:$G$4</c:f>
+              <c:f>'Execution Times'!$G$2:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>6.1160000000000001E-4</c:v>
                 </c:pt>
@@ -1349,6 +1553,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.9210000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.616E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7799999999999995E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1400,10 +1610,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Execution Times'!$H$2:$H$4</c:f>
+              <c:f>'Execution Times'!$H$2:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>5.6780000000000003E-4</c:v>
                 </c:pt>
@@ -1412,6 +1622,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.8570000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9200000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3600000000000001E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3873,16 +4089,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>65722</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>40565</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>153464</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>360045</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>92392</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285414</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>6555</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3909,16 +4125,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>391477</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>94297</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>382176</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>109312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>94297</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>120967</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>680813</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>134077</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4243,10 +4459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4261,117 +4477,281 @@
     <col min="8" max="8" customWidth="true" width="19.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>2.74994E-2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>2.4012100000000001E-2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>4.8685000000000004E-3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>3.4110009999999999E-3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="8">
         <v>7.8680000000000004E-4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>7.7220000000000001E-4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="9">
         <v>6.1160000000000001E-4</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="9">
         <v>5.6780000000000003E-4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>3.0609000000000001E-2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>2.32365E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>2.1538E-3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>1.9907000000000002E-3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="8">
         <v>7.3999999999999999E-4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="8">
         <v>7.4410000000000003E-4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="9">
         <v>1.5890000000000001E-4</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="9">
         <v>2.9499999999999999E-5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>3.5272400000000002E-2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>2.6511300000000002E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>9.2054000000000007E-3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>3.9805999999999999E-3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>1.008E-4</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>1.0450000000000001E-4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="9">
         <v>1.9210000000000001E-4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="9">
         <v>2.8570000000000001E-4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" t="n">
-        <v>0.0110049</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0042648</v>
-      </c>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2.7387600000000002E-2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2.2605699999999999E-2</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.10049E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4.2648E-3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>4.4400000000000002E-5</v>
+      </c>
+      <c r="F5" s="8">
+        <v>3.5800000000000003E-5</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1.616E-4</v>
+      </c>
+      <c r="H5" s="9">
+        <v>2.9200000000000002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>1.91285E-2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1.9986400000000001E-2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1.07534E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>5.0403000000000002E-3</v>
+      </c>
+      <c r="E6" s="8">
+        <v>7.47E-5</v>
+      </c>
+      <c r="F6" s="8">
+        <v>7.8100000000000001E-5</v>
+      </c>
+      <c r="G6" s="9">
+        <v>6.7799999999999995E-5</v>
+      </c>
+      <c r="H6" s="9">
+        <v>2.3600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7">
+        <v>8.4519999999999994E-3</v>
+      </c>
+      <c r="D7">
+        <v>3.9798000000000004E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.604E-4</v>
+      </c>
+      <c r="F7">
+        <v>1.01E-4</v>
+      </c>
+      <c r="G7" s="9">
+        <v>8.6600000000000004E-5</v>
+      </c>
+      <c r="H7" s="9">
+        <v>7.6199999999999995E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9">
+        <v>1.27E-4</v>
+      </c>
+      <c r="H8" s="9">
+        <v>9.31E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9">
+        <v>3.2100000000000001E-5</v>
+      </c>
+      <c r="H9" s="9">
+        <v>2.3499999999999999E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" t="n">
+        <v>7.09E-4</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5.68E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed memory calculation for sequential trees
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/SequentialExecutionTimes.xlsx
+++ b/src/main/resources/data_output/SequentialExecutionTimes.xlsx
@@ -480,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
@@ -1119,8 +1119,12 @@
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="G19" t="n">
+        <v>0.1154601</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.1431686</v>
+      </c>
       <c r="I19" t="n">
         <v>0.0010375</v>
       </c>
@@ -1145,8 +1149,12 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="G20" t="n">
+        <v>0.1081391</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.1331268</v>
+      </c>
       <c r="I20" t="n">
         <v>0.001406</v>
       </c>
@@ -1171,8 +1179,12 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="G21" t="n">
+        <v>0.0997361</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.1361017</v>
+      </c>
       <c r="I21" t="n">
         <v>0.0012484</v>
       </c>
@@ -1283,6 +1295,12 @@
       </c>
     </row>
     <row r="26">
+      <c r="I26" t="n">
+        <v>0.0231459</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.0147596</v>
+      </c>
       <c r="K26" t="n">
         <v>0.5881297</v>
       </c>
@@ -1296,6 +1314,14 @@
       </c>
       <c r="L27" t="n">
         <v>0.6250793</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="K28" t="n">
+        <v>0.6117588</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.5543064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>